<commit_message>
Combined Add_Vendor_Admin and Add_Vendor_Report into one script
</commit_message>
<xml_diff>
--- a/EasyVend Setup Scripts/Data.xlsx
+++ b/EasyVend Setup Scripts/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdagg\Documents\EasyVend Setup Scripts\EasyVend Setup Scripts\EasyVend Setup Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5610D9-76B7-4E2D-925B-CE7EE5C99F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB71129-50E9-43D9-8FE8-8028A22A2FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="-12735" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6885" yWindow="-14550" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>Email</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>Devices</t>
+  </si>
+  <si>
+    <t>eartha51@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Artha</t>
+  </si>
+  <si>
+    <t>pavel@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Avel</t>
+  </si>
+  <si>
+    <t>ethelmae235@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Thelmae</t>
   </si>
 </sst>
 </file>
@@ -480,15 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F11"/>
+  <dimension ref="A3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.88671875" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
@@ -655,6 +679,57 @@
       </c>
       <c r="F11" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>6612200748</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>6612200748</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <v>6612200748</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -667,6 +742,9 @@
     <hyperlink ref="A7" r:id="rId6" xr:uid="{797122D1-AA1D-4D4F-8282-94A2A20FD435}"/>
     <hyperlink ref="A8" r:id="rId7" xr:uid="{CC798E75-3B96-495F-B72D-497D90E044A5}"/>
     <hyperlink ref="A6" r:id="rId8" xr:uid="{0CFA6B23-91CA-4167-B1D5-2FA3EB80CF96}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{E72E39B8-8B8B-4448-8FD5-E98DC870228A}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{58176980-5AF9-4290-8BC7-28A71B942967}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{1047515D-99FE-451A-BA10-4C74BCBBF901}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -676,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F2098D-8E43-419C-868C-1D1CDE51B870}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
combined Add_Lottery_Admin and Add_Lottery_Report into one script
</commit_message>
<xml_diff>
--- a/EasyVend Setup Scripts/Data.xlsx
+++ b/EasyVend Setup Scripts/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdagg\Documents\EasyVend Setup Scripts\EasyVend Setup Scripts\EasyVend Setup Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB71129-50E9-43D9-8FE8-8028A22A2FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3971B6C5-B137-480F-8DCD-D460F0CA66D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6885" yWindow="-14550" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Email</t>
   </si>
@@ -176,6 +176,27 @@
   </si>
   <si>
     <t>Thelmae</t>
+  </si>
+  <si>
+    <t>samanyu5@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Amanyu</t>
+  </si>
+  <si>
+    <t>malia25@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Alia</t>
+  </si>
+  <si>
+    <t>samantha5@jolongestr.com</t>
   </si>
 </sst>
 </file>
@@ -504,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F14"/>
+  <dimension ref="A3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,6 +753,57 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <v>6612200748</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16">
+        <v>6612200748</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17">
+        <v>6612200748</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{833A3BBC-A753-4B2F-81CE-A7CE8F75D305}"/>
@@ -745,6 +817,9 @@
     <hyperlink ref="A12" r:id="rId9" xr:uid="{E72E39B8-8B8B-4448-8FD5-E98DC870228A}"/>
     <hyperlink ref="A13" r:id="rId10" xr:uid="{58176980-5AF9-4290-8BC7-28A71B942967}"/>
     <hyperlink ref="A14" r:id="rId11" xr:uid="{1047515D-99FE-451A-BA10-4C74BCBBF901}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{72968A25-A9CB-47A6-BF40-BF992A20FB51}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{D67E000E-07A9-4FD2-9140-F407BE7468A2}"/>
+    <hyperlink ref="A17" r:id="rId14" xr:uid="{1A0DBEB3-A7AB-437F-AB6F-0C56B8A8188E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added ability to add site user to multiple sites
</commit_message>
<xml_diff>
--- a/EasyVend Setup Scripts/Data.xlsx
+++ b/EasyVend Setup Scripts/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdagg\Documents\EasyVend Setup Scripts\EasyVend Setup Scripts\EasyVend Setup Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3971B6C5-B137-480F-8DCD-D460F0CA66D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA722E91-1076-4F52-8B37-D9679C9C21C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6885" yWindow="-14550" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7395" yWindow="-13500" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Email</t>
   </si>
@@ -49,60 +49,24 @@
     <t>Vendor Admin</t>
   </si>
   <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
     <t>Vendor Report</t>
   </si>
   <si>
-    <t>test3@email.com</t>
-  </si>
-  <si>
-    <t>Lottery</t>
-  </si>
-  <si>
     <t>Lottery Admin</t>
   </si>
   <si>
-    <t>test4@email.com</t>
-  </si>
-  <si>
     <t>Lottery Report</t>
   </si>
   <si>
-    <t>test5@email.com</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
     <t>Site Admin</t>
   </si>
   <si>
-    <t>test6@email.com</t>
-  </si>
-  <si>
     <t>Site Report</t>
   </si>
   <si>
-    <t>qrst@email.com</t>
-  </si>
-  <si>
-    <t>uvw@email.com</t>
-  </si>
-  <si>
-    <t>xyza@email.com</t>
-  </si>
-  <si>
-    <t>dfgfw@email.com</t>
-  </si>
-  <si>
     <t>Agent Number</t>
   </si>
   <si>
@@ -133,70 +97,94 @@
     <t>Chattsworth</t>
   </si>
   <si>
-    <t>Site 4565</t>
-  </si>
-  <si>
-    <t>Store 4565</t>
-  </si>
-  <si>
-    <t>Site 8753</t>
-  </si>
-  <si>
-    <t>Store 8753</t>
-  </si>
-  <si>
-    <t>Site 2374</t>
-  </si>
-  <si>
-    <t>Store 2374</t>
-  </si>
-  <si>
     <t>Devices</t>
   </si>
   <si>
-    <t>eartha51@jolongestr.com</t>
-  </si>
-  <si>
-    <t>Edward</t>
-  </si>
-  <si>
-    <t>Artha</t>
-  </si>
-  <si>
-    <t>pavel@jolongestr.com</t>
-  </si>
-  <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>Avel</t>
-  </si>
-  <si>
-    <t>ethelmae235@jolongestr.com</t>
-  </si>
-  <si>
-    <t>Thelmae</t>
-  </si>
-  <si>
-    <t>samanyu5@jolongestr.com</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Amanyu</t>
-  </si>
-  <si>
-    <t>malia25@jolongestr.com</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Alia</t>
-  </si>
-  <si>
-    <t>samantha5@jolongestr.com</t>
+    <t>Site 7331</t>
+  </si>
+  <si>
+    <t>Store 7331</t>
+  </si>
+  <si>
+    <t>Site 8723</t>
+  </si>
+  <si>
+    <t>Store 8723</t>
+  </si>
+  <si>
+    <t>Site 6524</t>
+  </si>
+  <si>
+    <t>Store 6524</t>
+  </si>
+  <si>
+    <t>tamara5@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Amara</t>
+  </si>
+  <si>
+    <t>pieter@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Ieter</t>
+  </si>
+  <si>
+    <t>bdazzledblue@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Dazzled</t>
+  </si>
+  <si>
+    <t>janne130@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>antwuan24@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Twuan</t>
+  </si>
+  <si>
+    <t>ceceilia3@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Ceilia</t>
+  </si>
+  <si>
+    <t>daimler@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Aimler</t>
+  </si>
+  <si>
+    <t>celines431@jolongestr.com</t>
+  </si>
+  <si>
+    <t>Eline</t>
+  </si>
+  <si>
+    <t>grgefe123</t>
   </si>
 </sst>
 </file>
@@ -525,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,286 +528,231 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>6612200748</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
+      <c r="A3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>6612200748</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>6612200748</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4">
-        <v>6612200748</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>6612200748</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>6612200748</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>6612200748</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>6612200748</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>6612200748</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
+      <c r="F8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>6612200748</v>
+      </c>
+      <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>6612200748</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
+      <c r="F9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>6612200748</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>6612200748</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12">
-        <v>6612200748</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13">
-        <v>6612200748</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14">
-        <v>6612200748</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15">
-        <v>6612200748</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16">
-        <v>6612200748</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17">
-        <v>6612200748</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{833A3BBC-A753-4B2F-81CE-A7CE8F75D305}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{ED564286-6655-4F23-BF15-C0270C75150A}"/>
-    <hyperlink ref="A10" r:id="rId3" xr:uid="{9939CF80-E93D-456C-B242-A455416D1E67}"/>
-    <hyperlink ref="A11" r:id="rId4" xr:uid="{B19F2184-5B08-4F5A-B1B8-7281BE7FA70E}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{2B45C9CE-34B7-41D5-B757-69DAF949A731}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{797122D1-AA1D-4D4F-8282-94A2A20FD435}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{CC798E75-3B96-495F-B72D-497D90E044A5}"/>
-    <hyperlink ref="A6" r:id="rId8" xr:uid="{0CFA6B23-91CA-4167-B1D5-2FA3EB80CF96}"/>
-    <hyperlink ref="A12" r:id="rId9" xr:uid="{E72E39B8-8B8B-4448-8FD5-E98DC870228A}"/>
-    <hyperlink ref="A13" r:id="rId10" xr:uid="{58176980-5AF9-4290-8BC7-28A71B942967}"/>
-    <hyperlink ref="A14" r:id="rId11" xr:uid="{1047515D-99FE-451A-BA10-4C74BCBBF901}"/>
-    <hyperlink ref="A15" r:id="rId12" xr:uid="{72968A25-A9CB-47A6-BF40-BF992A20FB51}"/>
-    <hyperlink ref="A16" r:id="rId13" xr:uid="{D67E000E-07A9-4FD2-9140-F407BE7468A2}"/>
-    <hyperlink ref="A17" r:id="rId14" xr:uid="{1A0DBEB3-A7AB-437F-AB6F-0C56B8A8188E}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4B15683D-C0F8-42F2-9250-8D37B5FB5E49}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{9E76F07A-125A-4127-99A2-E936FA9DC35B}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{6F7E2C91-5C2D-443D-A21F-5337F63D2B1D}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{FD95FF65-F5A5-4DAB-97A9-8F6FF0789A69}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{A5728647-CD87-4327-94D7-636A6DECA2E2}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{1E51F649-8736-4F98-9408-3824AA4BA382}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{7CDE9AB3-8FBB-4C77-AA8C-DFE0141BDB83}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{85C7F253-34E6-4F94-BB21-DB5E5D8ECF44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -827,10 +760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F2098D-8E43-419C-868C-1D1CDE51B870}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,20 +774,20 @@
     <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -869,33 +802,33 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>4565</v>
+        <v>7331</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -904,10 +837,10 @@
         <v>6612200748</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J2">
         <v>12345</v>
@@ -918,19 +851,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>8753</v>
+        <v>8723</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
@@ -939,33 +872,33 @@
         <v>6612200748</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J3">
         <v>12345</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>2374</v>
+        <v>6524</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
@@ -974,23 +907,29 @@
         <v>6612200748</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J4">
         <v>12345</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{97922FD7-ED43-41FA-8777-660DA5405780}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{CBD8E4A5-8D2C-4ECB-B50D-B505A5CFC3DE}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{75D34704-2E19-4141-BDFA-2C22B4C7CC09}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{75D34704-2E19-4141-BDFA-2C22B4C7CC09}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{97922FD7-ED43-41FA-8777-660DA5405780}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{CBD8E4A5-8D2C-4ECB-B50D-B505A5CFC3DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added support for adding devices to a site with external terminal Id and  serial number set in the excel file
</commit_message>
<xml_diff>
--- a/EasyVend Setup Scripts/Data.xlsx
+++ b/EasyVend Setup Scripts/Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdagg\Documents\EasyVend Setup Scripts\EasyVend Setup Scripts\EasyVend Setup Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\EasyVend TMS Setup Script\EasyVend Setup Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A790673-3519-46B8-8178-1BE81207C558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D213FA68-BC21-464E-9505-22EA8553FD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6465" yWindow="-12825" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34995" yWindow="1905" windowWidth="15420" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Sites" sheetId="3" r:id="rId2"/>
+    <sheet name="Devices" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
   <si>
     <t>Email</t>
   </si>
@@ -184,13 +185,253 @@
     <t>Excel Site3</t>
   </si>
   <si>
-    <t>ex1</t>
-  </si>
-  <si>
-    <t>ex2</t>
-  </si>
-  <si>
-    <t>ex3</t>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>TerminalId1</t>
+  </si>
+  <si>
+    <t>TerminalId2</t>
+  </si>
+  <si>
+    <t>TerminalId3</t>
+  </si>
+  <si>
+    <t>TerminalId4</t>
+  </si>
+  <si>
+    <t>Excel Site5</t>
+  </si>
+  <si>
+    <t>ex5</t>
+  </si>
+  <si>
+    <t>ex6</t>
+  </si>
+  <si>
+    <t>ex7</t>
+  </si>
+  <si>
+    <t>ex8</t>
+  </si>
+  <si>
+    <t>5a1</t>
+  </si>
+  <si>
+    <t>5a2</t>
+  </si>
+  <si>
+    <t>5a3</t>
+  </si>
+  <si>
+    <t>5a4</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>5b1</t>
+  </si>
+  <si>
+    <t>5b2</t>
+  </si>
+  <si>
+    <t>5b3</t>
+  </si>
+  <si>
+    <t>5b4</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>5c1</t>
+  </si>
+  <si>
+    <t>5c2</t>
+  </si>
+  <si>
+    <t>5c3</t>
+  </si>
+  <si>
+    <t>5c4</t>
+  </si>
+  <si>
+    <t>5d</t>
+  </si>
+  <si>
+    <t>5d1</t>
+  </si>
+  <si>
+    <t>5d2</t>
+  </si>
+  <si>
+    <t>5d3</t>
+  </si>
+  <si>
+    <t>5d4</t>
+  </si>
+  <si>
+    <t>Excel Site7</t>
+  </si>
+  <si>
+    <t>Excel Site8</t>
+  </si>
+  <si>
+    <t>Excel Site6</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>6a1</t>
+  </si>
+  <si>
+    <t>6a2</t>
+  </si>
+  <si>
+    <t>6a3</t>
+  </si>
+  <si>
+    <t>6a4</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>6b1</t>
+  </si>
+  <si>
+    <t>6b2</t>
+  </si>
+  <si>
+    <t>6b3</t>
+  </si>
+  <si>
+    <t>6b4</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>6c1</t>
+  </si>
+  <si>
+    <t>6c2</t>
+  </si>
+  <si>
+    <t>6c3</t>
+  </si>
+  <si>
+    <t>6c4</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>7a1</t>
+  </si>
+  <si>
+    <t>7a2</t>
+  </si>
+  <si>
+    <t>7a3</t>
+  </si>
+  <si>
+    <t>7a4</t>
+  </si>
+  <si>
+    <t>7b</t>
+  </si>
+  <si>
+    <t>7b1</t>
+  </si>
+  <si>
+    <t>7b2</t>
+  </si>
+  <si>
+    <t>7b3</t>
+  </si>
+  <si>
+    <t>7b4</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>8a1</t>
+  </si>
+  <si>
+    <t>8a2</t>
+  </si>
+  <si>
+    <t>8a3</t>
+  </si>
+  <si>
+    <t>8a4</t>
+  </si>
+  <si>
+    <t>8b1</t>
+  </si>
+  <si>
+    <t>8b2</t>
+  </si>
+  <si>
+    <t>8b3</t>
+  </si>
+  <si>
+    <t>8b4</t>
+  </si>
+  <si>
+    <t>8c1</t>
+  </si>
+  <si>
+    <t>8c2</t>
+  </si>
+  <si>
+    <t>8c3</t>
+  </si>
+  <si>
+    <t>8c4</t>
+  </si>
+  <si>
+    <t>8d1</t>
+  </si>
+  <si>
+    <t>8d2</t>
+  </si>
+  <si>
+    <t>8d3</t>
+  </si>
+  <si>
+    <t>8d4</t>
+  </si>
+  <si>
+    <t>8f1</t>
+  </si>
+  <si>
+    <t>8f2</t>
+  </si>
+  <si>
+    <t>8f3</t>
+  </si>
+  <si>
+    <t>8f4</t>
+  </si>
+  <si>
+    <t>8g1</t>
+  </si>
+  <si>
+    <t>8g2</t>
+  </si>
+  <si>
+    <t>8g3</t>
+  </si>
+  <si>
+    <t>8g4</t>
   </si>
 </sst>
 </file>
@@ -521,21 +762,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -572,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -589,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -606,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -623,7 +864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -643,7 +884,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -663,7 +904,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -683,7 +924,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -703,7 +944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -723,7 +964,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -743,7 +984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -763,25 +1004,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
   </sheetData>
@@ -807,23 +1048,23 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -858,15 +1099,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -890,18 +1131,18 @@
         <v>12345</v>
       </c>
       <c r="K2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -928,15 +1169,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -960,16 +1201,48 @@
         <v>12345</v>
       </c>
       <c r="K4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>6612200748</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>12345</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
     </row>
   </sheetData>
@@ -977,7 +1250,336 @@
     <hyperlink ref="F4" r:id="rId1" xr:uid="{75D34704-2E19-4141-BDFA-2C22B4C7CC09}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{97922FD7-ED43-41FA-8777-660DA5405780}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{CBD8E4A5-8D2C-4ECB-B50D-B505A5CFC3DE}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{3603056F-26BC-4BBC-BC0F-8AFEBFF767F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1896FEA1-3EBE-4464-8A3C-C90A79E5BFC3}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>